<commit_message>
preparing carb analysis and calibration curve
</commit_message>
<xml_diff>
--- a/Lab measurements 0515.xlsx
+++ b/Lab measurements 0515.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\ACES\Dissy\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\OneDrive\Documents\GitHub\TEdissy_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03945469-8F32-456E-9E8E-ABABFCEF7865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F61C63-54BB-44C0-8721-A378A7EAB7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" activeTab="4" xr2:uid="{240FB520-7280-45DA-A7FE-A0684635DDBB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="8" xr2:uid="{240FB520-7280-45DA-A7FE-A0684635DDBB}"/>
   </bookViews>
   <sheets>
     <sheet name="proteins" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="363">
   <si>
     <t>sample weight</t>
   </si>
@@ -7365,7 +7365,7 @@
   <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9290,7 +9290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4237F4E7-1628-446A-9D84-1DC2D76134A6}">
   <dimension ref="A1:F189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -14973,18 +14973,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CE3D234-D121-4271-A8AF-3A7A4B05AD00}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -14992,319 +14989,202 @@
         <v>351</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2">
         <v>4.3</v>
       </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="1">
-        <v>45793</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3">
         <v>4.7E-2</v>
       </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="1">
-        <v>45793</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="1">
-        <v>45793</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="1">
-        <v>45793</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="1">
-        <v>45793</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
         <v>7.3</v>
       </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="1">
-        <v>45793</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8">
         <v>4.3</v>
       </c>
-      <c r="C8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="1">
-        <v>45793</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9">
         <v>4.2</v>
       </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="1">
-        <v>45793</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10">
         <v>5.5</v>
       </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="1">
-        <v>45793</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11">
         <v>5.3</v>
       </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="1">
-        <v>45793</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="1">
-        <v>45793</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="1">
-        <v>45793</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15">
         <v>5.2</v>
       </c>
-      <c r="C15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16">
         <v>6.1</v>
       </c>
-      <c r="C16" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
       <c r="B17">
         <v>6.8</v>
       </c>
-      <c r="C17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18">
         <v>6.2</v>
       </c>
-      <c r="C18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19">
         <v>6.3</v>
       </c>
-      <c r="C19" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
       <c r="B20">
         <v>5.3</v>
       </c>
-      <c r="C20" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21">
         <v>4.3</v>
       </c>
-      <c r="C21" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
       <c r="B22">
         <v>6.1</v>
       </c>
-      <c r="C22" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>29</v>
       </c>
       <c r="B23">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>30</v>
       </c>
       <c r="B24">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -15312,7 +15192,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -15320,7 +15200,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -15328,7 +15208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -15336,7 +15216,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -15344,7 +15224,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -15352,7 +15232,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>140</v>
       </c>

</xml_diff>